<commit_message>
- revamp Excel handling to improve performance.
[json]
- [`assertEqual(expected,actual)`](../commands/json/assertEqual(expected,actual))): enhanced with better message to aid in troubleshooting.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_IterationDataTests.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_IterationDataTests.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B05FC4D-BB95-E942-9E0D-BF7F8E6E4FDF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E494C7-3E04-3D45-BAAF-32343A2AB551}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="23440" windowHeight="9320" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="23440" windowHeight="9320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:AAA10"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A2DE7A-75FB-754E-A597-C54034E3E50F}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2310,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC721390-C655-0A47-ADAC-091E91553666}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>